<commit_message>
Update file mẫu import cán bộ
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/canbo.xlsx
+++ b/Sources/DD_RFID/public/download/canbo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>MSCB</t>
   </si>
@@ -170,6 +170,114 @@
       </rPr>
       <t>: Lưu file mẫu lại. Quay lại giao diện quản lý cán bộ.</t>
     </r>
+  </si>
+  <si>
+    <t>00123456</t>
+  </si>
+  <si>
+    <t>Nguyễn Ân Hiên</t>
+  </si>
+  <si>
+    <t>vana@gmail.com</t>
+  </si>
+  <si>
+    <t>00123457</t>
+  </si>
+  <si>
+    <t>Trần Văn Bình</t>
+  </si>
+  <si>
+    <t>vanb@gmail.com</t>
+  </si>
+  <si>
+    <t>00123458</t>
+  </si>
+  <si>
+    <t>Phan Công Huy</t>
+  </si>
+  <si>
+    <t>pchuy@gmail.com</t>
+  </si>
+  <si>
+    <t>00123459</t>
+  </si>
+  <si>
+    <t>Lê Thị Hậu</t>
+  </si>
+  <si>
+    <t>hau@hotmail.com</t>
+  </si>
+  <si>
+    <t>00123460</t>
+  </si>
+  <si>
+    <t>Nguyễn Chín</t>
+  </si>
+  <si>
+    <t>chin@email.com</t>
+  </si>
+  <si>
+    <t>00123461</t>
+  </si>
+  <si>
+    <t>Lê Thành Công</t>
+  </si>
+  <si>
+    <t>cong@outlook.com</t>
+  </si>
+  <si>
+    <t>00123462</t>
+  </si>
+  <si>
+    <t>Phương Tín</t>
+  </si>
+  <si>
+    <t>Ptin@gmail.com.vn</t>
+  </si>
+  <si>
+    <t>00123463</t>
+  </si>
+  <si>
+    <t>Lâm Định Cương</t>
+  </si>
+  <si>
+    <t>ldcuong@gmail.com</t>
+  </si>
+  <si>
+    <t>00123464</t>
+  </si>
+  <si>
+    <t>Mai Ất Nguyên</t>
+  </si>
+  <si>
+    <t>nguyenmaiat@gmail.com</t>
+  </si>
+  <si>
+    <t>00123465</t>
+  </si>
+  <si>
+    <t>Phạm Thắng</t>
+  </si>
+  <si>
+    <t>thangthang@gmail.com.vn</t>
+  </si>
+  <si>
+    <t>00123466</t>
+  </si>
+  <si>
+    <t>Trương Tuấn Kiên</t>
+  </si>
+  <si>
+    <t>tkien@yahoo.com.vn</t>
+  </si>
+  <si>
+    <t>00123467</t>
+  </si>
+  <si>
+    <t>Đinh Phùng Quân</t>
+  </si>
+  <si>
+    <t>phungquan@gmail.com.vn</t>
   </si>
 </sst>
 </file>
@@ -1942,7 +2050,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,55 +2080,209 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Cập nhật chức năng kiếm tra định dạng file trước khi import.
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/canbo.xlsx
+++ b/Sources/DD_RFID/public/download/canbo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hướng dẫn sử dụng" sheetId="4" r:id="rId1"/>
@@ -1035,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -2309,7 +2309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Hoàn thành import sinh viên
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/canbo.xlsx
+++ b/Sources/DD_RFID/public/download/canbo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>MSCB</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>- Sheet 'data' dùng để tham chiếu giá trị các bộ môn và tên khoa, chỉ bổ sung khi cần.</t>
+  </si>
+  <si>
+    <t>TÊN KHOA</t>
+  </si>
+  <si>
+    <t>TÊN BỘ MÔN</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1042,7 @@
   <dimension ref="B3:Q56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1069,7 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2050,7 +2056,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2293,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>KHOA</formula1>
     </dataValidation>
     <dataValidation type="textLength" errorStyle="information" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Lỗi dữ liệu" error="Mã số phải là 8 kí tự." sqref="A1:A1048576">
@@ -2296,7 +2302,7 @@
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lỗi dữ liệu" error="Họ tên tối đa 50 ký tự." sqref="B1:B1048576">
       <formula1>50</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lỗi dữ liệu" error="Nên dùng tên bộ môn trong danh sách có sẳn." sqref="C1:C1048576 C1">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lỗi dữ liệu" error="Nên dùng tên bộ môn trong danh sách có sẳn." sqref="C2:C1048576">
       <formula1>BOMON</formula1>
     </dataValidation>
   </dataValidations>
@@ -2310,7 +2316,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,10 +2327,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>